<commit_message>
finished leaflet and added text
</commit_message>
<xml_diff>
--- a/data/ukdict.xlsx
+++ b/data/ukdict.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tinatsou/Documents/semester2/ETC5523 Communicating with Data/blog-ttsou87/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2F5E68-0B32-3B4F-A271-4F66A53BA24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA790308-A9C5-E248-A376-3972ABB05B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="7800" windowWidth="24160" windowHeight="10200" activeTab="1" xr2:uid="{A271C9CA-23AE-4C57-A900-DFBE670992A5}"/>
+    <workbookView xWindow="10280" yWindow="5440" windowWidth="24160" windowHeight="10200" activeTab="2" xr2:uid="{A271C9CA-23AE-4C57-A900-DFBE670992A5}"/>
   </bookViews>
   <sheets>
     <sheet name="ukcase" sheetId="6" r:id="rId1"/>
-    <sheet name="state_milk_production" sheetId="5" r:id="rId2"/>
+    <sheet name="ukvacc" sheetId="5" r:id="rId2"/>
+    <sheet name="englandvacc" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>variable</t>
   </si>
@@ -93,6 +94,66 @@
   </si>
   <si>
     <t>Cumulative percentage of population age 16 and above with the two doses of vaccine</t>
+  </si>
+  <si>
+    <t>areaCode</t>
+  </si>
+  <si>
+    <t>areaName</t>
+  </si>
+  <si>
+    <t>areaType</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>Completely Vaccinated</t>
+  </si>
+  <si>
+    <t>First Dose</t>
+  </si>
+  <si>
+    <t>Second Dose</t>
+  </si>
+  <si>
+    <t>pop</t>
+  </si>
+  <si>
+    <t>firstperc</t>
+  </si>
+  <si>
+    <t>secondperc</t>
+  </si>
+  <si>
+    <t>Area code of the region</t>
+  </si>
+  <si>
+    <t>Name of the region</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Date of data publication</t>
+  </si>
+  <si>
+    <t>Total number of people fully vaccinated</t>
+  </si>
+  <si>
+    <t>Total number of people with one dose of vaccine</t>
+  </si>
+  <si>
+    <t>Total number of people with two doses of vaccines</t>
+  </si>
+  <si>
+    <t>Population of the region (2020)</t>
+  </si>
+  <si>
+    <t>Percentage of population with first dose</t>
+  </si>
+  <si>
+    <t>Percentage of population with two doses</t>
   </si>
 </sst>
 </file>
@@ -538,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1010590-69BB-4481-B9B8-8AEB5184DB74}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -596,4 +657,144 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC4E145-991B-9946-BF3C-13CDB109FAB9}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>